<commit_message>
Updated Ethiopia with fixed Cattle regional parameters
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/Subnational parameters/BG 2021_AHLE scenario parameters CATTLE scenarios only.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/Subnational parameters/BG 2021_AHLE scenario parameters CATTLE scenarios only.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADsLiverpool\Ethiopia Workspace\Code and Control Files\Subnational parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0938C310-32BA-4D53-BF7F-F30448F6706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3E8877-7C92-4396-9807-2631A1478C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="14292" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1644,10 +1644,10 @@
     <t>rpert(10000, (920.52/12), (920.52/12), (920.52/12))</t>
   </si>
   <si>
-    <t>rpert(10000, (2675), (15591), (6000))</t>
-  </si>
-  <si>
     <t>rpert(10000, (2.19*12.5*0.9515), (9*12.5*0.9515), (5.4*12.5*0.9515))</t>
+  </si>
+  <si>
+    <t>rpert(10000, (6000), (26750), (15591))</t>
   </si>
 </sst>
 </file>
@@ -5738,7 +5738,7 @@
         <v>210</v>
       </c>
       <c r="E73" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>210</v>
@@ -5765,7 +5765,7 @@
         <v>210</v>
       </c>
       <c r="N73" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O73" s="14" t="s">
         <v>210</v>
@@ -6094,49 +6094,49 @@
         <v>106</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q84" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="R84" s="18"/>
       <c r="S84" s="18"/>

</xml_diff>